<commit_message>
complete celery scheduled task
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VS Code Projects\restaurant-fastapi\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63D61A6-47C1-4EF8-A374-41108CCCA8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4C9BD8-5E16-4070-886D-A9546EF25C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Меню</t>
   </si>
@@ -133,9 +133,6 @@
   </si>
   <si>
     <t>Нарезка из ветчины, колбасных колечек, нескольких сортов сыра и фруктов</t>
-  </si>
-  <si>
-    <t>3.5%</t>
   </si>
 </sst>
 </file>
@@ -488,7 +485,9 @@
   </sheetPr>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="14.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -688,7 +687,7 @@
       <c r="G11" s="9"/>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:10" ht="15.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2">
@@ -703,8 +702,8 @@
       <c r="F12" s="7">
         <v>2700.79</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>36</v>
+      <c r="G12" s="9">
+        <v>0.04</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.8" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>